<commit_message>
CiAn: updated list of materials
</commit_message>
<xml_diff>
--- a/Master_ETTI_M21_and_M25_Course_Structure_and_OIL.xlsx
+++ b/Master_ETTI_M21_and_M25_Course_Structure_and_OIL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6336" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6336"/>
   </bookViews>
   <sheets>
     <sheet name="NecesarMateriale" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
   <si>
     <t>System Concepts</t>
   </si>
@@ -219,9 +219,6 @@
     <t>Nr.</t>
   </si>
   <si>
-    <t xml:space="preserve">PC-uri cu Windows 7 </t>
-  </si>
-  <si>
     <t>Licente TargetLink</t>
   </si>
   <si>
@@ -231,12 +228,6 @@
     <t>Pret</t>
   </si>
   <si>
-    <t>Placute pentru Embedded Coder</t>
-  </si>
-  <si>
-    <t>Periferice/systeme demonstrative conectate cu placuta</t>
-  </si>
-  <si>
     <t>M21. Vehicle Control Systems</t>
   </si>
   <si>
@@ -249,12 +240,6 @@
     <t>Licente Matlab cu Embedded Coder, Simulink, Stateflow, Control System</t>
   </si>
   <si>
-    <t>Optional: Simscape with SimElectronics and SimPower Systems</t>
-  </si>
-  <si>
-    <t>Aparate de masura (surse, osciloscop, generatoare de semanl etc.)</t>
-  </si>
-  <si>
     <t>Materiale necesare M21-M25</t>
   </si>
   <si>
@@ -274,13 +259,31 @@
   </si>
   <si>
     <t>Have a first initial draft curicula</t>
+  </si>
+  <si>
+    <t>PC-uri cu Windows 7 / Windows 10</t>
+  </si>
+  <si>
+    <t>Optional: Simscape with SimElectronics and SimPower Systems, Signal Processing</t>
+  </si>
+  <si>
+    <t>Placute pentru Embedded Coder (NUCLEO-L496ZG)</t>
+  </si>
+  <si>
+    <t>Motor (to be decided type and invertor if needed)</t>
+  </si>
+  <si>
+    <t>Sursa tensiune (minim 20A, 20V)</t>
+  </si>
+  <si>
+    <t>Osciloscoape</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +293,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -332,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -346,6 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D9"/>
+  <dimension ref="B1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,18 +651,18 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -658,7 +670,7 @@
     </row>
     <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -666,50 +678,58 @@
     </row>
     <row r="4" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>60</v>
+      <c r="B5" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>61</v>
+      <c r="B6" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -723,7 +743,7 @@
   <dimension ref="A2:F33"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,7 +771,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -905,7 +925,7 @@
     </row>
     <row r="19" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>0</v>
@@ -1053,7 +1073,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1069,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,7 +1215,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
         <v>53</v>
@@ -1212,7 +1232,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
         <v>53</v>
@@ -1229,7 +1249,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
         <v>49</v>
@@ -1246,7 +1266,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>53</v>
@@ -1263,7 +1283,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
         <v>49</v>
@@ -1280,7 +1300,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
CiAn: update list of materials after synchronization meeting
</commit_message>
<xml_diff>
--- a/Master_ETTI_M21_and_M25_Course_Structure_and_OIL.xlsx
+++ b/Master_ETTI_M21_and_M25_Course_Structure_and_OIL.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
   <si>
     <t>System Concepts</t>
   </si>
@@ -277,6 +277,21 @@
   </si>
   <si>
     <t>Osciloscoape</t>
+  </si>
+  <si>
+    <t>Breadboard + fire</t>
+  </si>
+  <si>
+    <t>Cabluri USB  (T-T) pentru placute Embedded Coder</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Solutie de backup pentru placute</t>
+  </si>
+  <si>
+    <t>To be decided</t>
   </si>
 </sst>
 </file>
@@ -308,12 +323,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -343,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -358,11 +391,43 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -638,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D10"/>
+  <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,87 +714,110 @@
     <col min="2" max="2" width="47.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>73</v>
       </c>
       <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
         <v>75</v>
       </c>
       <c r="C7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="C9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>77</v>
       </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>78</v>
       </c>
-      <c r="C10">
-        <v>10</v>
+      <c r="C11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1087,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1103,22 +1191,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1312,8 +1400,30 @@
         <v>54</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1">
+        <v>42962</v>
+      </c>
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F12"/>
+  <conditionalFormatting sqref="E2:E50">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"ongoing"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>